<commit_message>
Add BOL in stage
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageOrdersTestData.xlsx
+++ b/testdata/FCfiles/qa/ManageOrdersTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>Location Name</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>51485955</t>
+  </si>
+  <si>
+    <t>51529775</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
@@ -307,6 +310,7 @@
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -851,8 +855,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="43" t="s">
-        <v>66</v>
+      <c r="A2" s="46" t="s">
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>

</xml_diff>